<commit_message>
these is the commit
</commit_message>
<xml_diff>
--- a/College_Timetables.xlsx
+++ b/College_Timetables.xlsx
@@ -10,12 +10,12 @@
     <sheet name="Year2_DivA" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Year2_DivB" sheetId="2" state="visible" r:id="rId2"/>
     <sheet name="Year2_DivC" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Year2_DivD" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="Year3_DivA" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="Year3_DivB" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet name="Year3_DivC" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet name="Year4_DivA" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet name="Year4_DivB" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="Year3_DivA" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="Year3_DivB" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="Year3_DivC" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="Year4_DivA" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="Year4_DivB" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="Year4_DivC" sheetId="9" state="visible" r:id="rId9"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -444,42 +444,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -511,24 +511,20 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
+          <t>Computer Organization (theory) - F013 - R102</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Programming in Java (theory) - F014 - R101</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R101</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -538,14 +534,14 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>Data Structures (theory) - F001 - R101</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
           <t>Digital Logic Design (theory) - F002 - R101</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Data Structures (theory) - F001 - R101</t>
-        </is>
-      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -558,24 +554,20 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (theory) - F013 - R101</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Programming in Java (theory) - F014 - R101</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R102</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -590,39 +582,35 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Digital Logic Design (theory) - F002 - R102</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Lunch Break</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>Mathematics III (theory) - F003 - R101</t>
         </is>
       </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Computer Organization (theory) - F013 - R101</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Programming in Java (theory) - F014 - R101</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -637,7 +625,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Digital Logic Design (practical) - F002 - R201</t>
+          <t>Data Structures (practical) - F001 - R201 (cont.)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -647,29 +635,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Mathematics III (theory) - F003 - R102</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R101</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -679,12 +655,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Digital Logic Design (practical) - F002 - R201</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Digital Logic Design (practical) - F002 - R201 (cont.)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -694,29 +670,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R102</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -726,12 +690,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (practical) - F013 - R201</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (practical) - F013 - R201 (cont.)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -739,31 +703,11 @@
           <t>Lunch Break</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -787,42 +731,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -849,29 +793,21 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (theory) - F013 - R102</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
+          <t>Mathematics III (theory) - F003 - R101</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R102</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -881,12 +817,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Mathematics III (theory) - F003 - AUD1</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Digital Logic Design (practical) - F002 - R201</t>
+          <t>Discrete Mathematics (theory) - F015 - AUD1</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -901,24 +837,12 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Data Structures (practical) - F001 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -928,12 +852,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Discrete Mathematics (theory) - F015 - AUD1</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -941,31 +865,19 @@
           <t>Lunch Break</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
-        </is>
-      </c>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Digital Logic Design (practical) - F002 - R201</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Digital Logic Design (practical) - F002 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -975,12 +887,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - R102</t>
+          <t>Digital Logic Design (theory) - F002 - R101</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (theory) - F013 - R102</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -990,29 +902,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Programming in Java (theory) - F014 - AUD1</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Computer Organization (practical) - F013 - R201</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Computer Organization (practical) - F013 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1027,7 +931,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Digital Logic Design (theory) - F002 - R102</t>
+          <t>Mathematics III (theory) - F003 - R102</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1037,29 +941,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - R101</t>
+          <t>Computer Organization (theory) - F013 - R101</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Programming in Java (theory) - F014 - R102</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1069,12 +965,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Data Structures (theory) - F001 - R101</t>
+          <t>Data Structures (theory) - F001 - R102</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Digital Logic Design (theory) - F002 - R101</t>
+          <t>Digital Logic Design (theory) - F002 - R102</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1089,24 +985,16 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Programming in Java (theory) - F014 - R102</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R101</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1130,42 +1018,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -1177,14 +1065,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - AUD1</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Programming in Java (theory) - F014 - AUD1</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -1192,29 +1076,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Data Structures (practical) - F001 - R201</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Data Structures (practical) - F001 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1224,12 +1096,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - R102</t>
+          <t>Digital Logic Design (theory) - F002 - R102</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
+          <t>Computer Organization (theory) - F013 - R102</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1239,29 +1111,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Digital Logic Design (practical) - F002 - R202</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Digital Logic Design (practical) - F002 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Programming in Java (theory) - F014 - R101</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1271,44 +1135,40 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Digital Logic Design (theory) - F002 - R102</t>
+          <t>Mathematics III (theory) - F003 - R102</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Data Structures (theory) - F001 - R101</t>
         </is>
       </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Lunch Break</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - R101</t>
+          <t>Computer Organization (theory) - F013 - R102</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Programming in Java (theory) - F014 - R102</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R102</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1318,14 +1178,14 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>Mathematics III (theory) - F003 - R102</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
           <t>Digital Logic Design (theory) - F002 - R101</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Data Structures (theory) - F001 - R101</t>
-        </is>
-      </c>
       <c r="D5" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -1333,29 +1193,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Discrete Mathematics (theory) - F015 - R301</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Programming in Java (practical) - F014 - R202</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Programming in Java (practical) - F014 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1365,7 +1217,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Digital Logic Design (theory) - F002 - R102</t>
+          <t>Mathematics III (theory) - F003 - R102</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -1378,31 +1230,23 @@
           <t>Lunch Break</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Organization (theory) - F013 - R101</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Discrete Mathematics (theory) - F015 - R101</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Environmental Studies (NEP) (theory) - F010 - R101</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1412,12 +1256,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Digital Logic Design (practical) - F002 - R201</t>
+          <t>Digital Logic Design (theory) - F002 - AUD1</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Data Structures (practical) - F001 - R201</t>
+          <t>Data Structures (theory) - F001 - R101</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1427,29 +1271,25 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Discrete Mathematics (theory) - F015 - R102</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Mathematics III (theory) - F003 - R101</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Computer Organization (practical) - F013 - R201</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Computer Organization (practical) - F013 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1473,42 +1313,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -1520,12 +1360,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - R301</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (theory) - F005 - R301</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -1535,29 +1375,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - AUD1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Data Structures (theory) - F001 - R101</t>
+          <t>Software Engineering (theory) - F017 - R301</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Algorithms (theory) - F018 - AUD1</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - R102</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1567,12 +1403,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - R301</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
+          <t>Database Systems (theory) - F005 - R301</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1582,29 +1418,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - R102</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - R102</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Algorithms (theory) - F018 - AUD1</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Data Structures (theory) - F001 - R101</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - AUD1</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1614,12 +1446,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - R301</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (theory) - F005 - AUD1</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -1629,29 +1461,25 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - AUD1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - AUD1</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Algorithms (theory) - F018 - AUD1</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - AUD1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -1661,12 +1489,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (practical) - F004 - R202</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Mathematics III (theory) - F003 - R102</t>
+          <t>Operating Systems (practical) - F004 - R202 (cont.)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -1676,29 +1504,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>OE - Environmental Studies (theory) - F010 - AUD1</t>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Algorithms (theory) - F018 - AUD1</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -1708,12 +1524,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (practical) - F005 - R202</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (practical) - F005 - R202 (cont.)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -1721,31 +1537,11 @@
           <t>Lunch Break</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="E6" t="inlineStr"/>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -1755,12 +1551,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (practical) - F006 - R202</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (practical) - F006 - R202 (cont.)</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -1768,31 +1564,15 @@
           <t>Lunch Break</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+      <c r="E7" t="inlineStr"/>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1816,42 +1596,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -1863,7 +1643,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (theory) - F005 - AUD2</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -1878,29 +1658,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - AUD1</t>
+          <t>Algorithms (theory) - F018 - R301</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - AUD1</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Software Engineering (practical) - F017 - R201</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - R101</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Software Engineering (practical) - F017 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -1910,12 +1686,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - AUD1</t>
+          <t>Algorithms (theory) - F018 - AUD3</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
+          <t>Web Development (theory) - F019 - AUD3</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -1925,29 +1701,17 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - R102</t>
+          <t>Operating Systems (practical) - F004 - CL1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>OE - Constitution of India (theory) - F011 - AUD1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Operating Systems (practical) - F004 - CL1 (cont.)</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -1955,16 +1719,8 @@
           <t>Wed</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Operating Systems (theory) - F004 - AUD1</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -1972,29 +1728,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
+          <t>Database Systems (practical) - F005 - R201</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Computer Networks (theory) - F006 - R101</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>OE - Constitution of India (theory) - F011 - AUD1</t>
-        </is>
-      </c>
+          <t>Database Systems (practical) - F005 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2004,12 +1748,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Operating Systems (practical) - F004 - R202</t>
+          <t>Database Systems (theory) - F005 - AUD1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Database Systems (practical) - F005 - R202</t>
+          <t>Computer Networks (theory) - F006 - R301</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2019,29 +1763,25 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Computer Networks (practical) - F006 - R201</t>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - R102</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Computer Networks (practical) - F006 - CL1</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Computer Networks (practical) - F006 - CL1 (cont.)</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2051,12 +1791,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - AUD1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - R301</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2066,29 +1806,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - AUD1</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Algorithms (theory) - F018 - AUD1</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - R102</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2098,12 +1830,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - R301</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (theory) - F005 - R301</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2113,29 +1845,25 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - AUD1</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Algorithms (theory) - F018 - AUD1</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Web Development (theory) - F019 - R102</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2159,42 +1887,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -2206,14 +1934,10 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - AUD3</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -2221,29 +1945,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - R102</t>
+          <t>Operating Systems (practical) - F004 - R202</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Computer Networks (theory) - F006 - R101</t>
-        </is>
-      </c>
+          <t>Operating Systems (practical) - F004 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2253,12 +1965,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Database Systems (practical) - F005 - R201</t>
+          <t>Database Systems (theory) - F005 - AUD2</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Operating Systems (practical) - F004 - R202</t>
+          <t>Computer Networks (theory) - F006 - AUD2</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2268,29 +1980,21 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (practical) - F005 - CL2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Computer Networks (practical) - F006 - R201</t>
+          <t>Database Systems (practical) - F005 - CL2 (cont.)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>OE - Constitution of India (theory) - F011 - AUD1</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Software Engineering (theory) - F017 - R102</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2300,12 +2004,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Computer Networks (theory) - F006 - AUD2</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Operating Systems (theory) - F004 - R102</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2315,29 +2019,25 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - R301</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Algorithms (theory) - F018 - R301</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Computer Networks (practical) - F006 - R202</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>OE - Constitution of India (theory) - F011 - AUD1</t>
-        </is>
-      </c>
+          <t>Computer Networks (practical) - F006 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2347,12 +2047,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Software Engineering (theory) - F017 - R301</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Database Systems (theory) - F005 - AUD1</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2362,29 +2062,25 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Web Development (theory) - F019 - R301</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Algorithms (theory) - F018 - R101</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Web Development (theory) - F019 - R101</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2394,14 +2090,14 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>Computer Networks (theory) - F006 - R301</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
           <t>Operating Systems (theory) - F004 - AUD1</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
       <c r="D6" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -2409,29 +2105,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Computer Networks (theory) - F006 - R102</t>
-        </is>
-      </c>
+          <t>Algorithms (theory) - F018 - R301</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Software Engineering (practical) - F017 - R201</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Software Engineering (practical) - F017 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2441,12 +2129,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - R102</t>
+          <t>Database Systems (theory) - F005 - AUD2</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
+          <t>Operating Systems (theory) - F004 - AUD1</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2456,29 +2144,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - R102</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Algorithms (theory) - F018 - R301</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr"/>
+      <c r="G7" t="inlineStr"/>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>OE - Constitution of India (NEP) (theory) - F011 - R101</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2502,42 +2178,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -2549,12 +2225,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD4</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD3</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2564,29 +2240,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - CL2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - CL2 (cont.)</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Artificial Intelligence (theory) - F021 - R301</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>OE - Constitution of India (theory) - F011 - R102</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Big Data Analytics (theory) - F022 - AUD1</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2596,12 +2268,12 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD4</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD4</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -2611,29 +2283,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - LAB2</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - LAB2 (cont.)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Artificial Intelligence (theory) - F021 - R301</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Big Data Analytics (theory) - F022 - R301</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2643,12 +2311,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD3</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - AUD1</t>
+          <t>Cloud Computing (theory) - F008 - AUD2</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -2658,29 +2326,21 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - AUD1</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD2</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - R102</t>
+          <t>Big Data Analytics (theory) - F022 - AUD2</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -2690,12 +2350,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Database Systems (theory) - F005 - AUD1</t>
+          <t>Machine Learning (practical) - F007 - CL1</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - AUD1</t>
+          <t>Machine Learning (practical) - F007 - CL1 (cont.)</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -2705,29 +2365,17 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - R101</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>OE - Constitution of India (theory) - F011 - R101</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - AUD3</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr"/>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -2737,12 +2385,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (practical) - F008 - CL1</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Operating Systems (theory) - F004 - AUD1</t>
+          <t>Cloud Computing (practical) - F008 - CL1 (cont.)</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -2752,29 +2400,17 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Computer Networks (theory) - F006 - AUD1</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>Database Systems (theory) - F005 - R101</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr"/>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -2784,12 +2420,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Database Systems (practical) - F005 - R202</t>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Operating Systems (practical) - F004 - R202</t>
+          <t>Cyber Security (theory) - F023 - AUD4</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -2799,29 +2435,17 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Artificial Intelligence (practical) - F021 - R201</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Computer Networks (practical) - F006 - R201</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Artificial Intelligence (practical) - F021 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr"/>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -2845,42 +2469,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -2890,14 +2514,10 @@
           <t>Mon</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Major Project (practical) - F009 - R202</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R201</t>
+          <t>Machine Learning (theory) - F007 - AUD2</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -2907,29 +2527,25 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD2</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD2</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>Machine Learning (theory) - F007 - AUD1</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Cloud Computing (theory) - F008 - AUD1</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - R301</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -2937,16 +2553,8 @@
           <t>Tue</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Major Project (practical) - F009 - CL1</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -2954,29 +2562,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Machine Learning (theory) - F007 - AUD1</t>
+          <t>Machine Learning (practical) - F007 - LAB_BIG</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MDM - Seminar (theory) - F012 - AUD1</t>
+          <t>Machine Learning (practical) - F007 - LAB_BIG (cont.)</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Cloud Computing (theory) - F008 - R102</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -2984,16 +2588,8 @@
           <t>Wed</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Major Project (practical) - F009 - R201</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+      <c r="B4" t="inlineStr"/>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -3001,29 +2597,17 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (practical) - F008 - R202</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>Machine Learning (theory) - F007 - R102</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Cloud Computing (theory) - F008 - R101</t>
-        </is>
-      </c>
+          <t>Cloud Computing (practical) - F008 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr"/>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3033,12 +2617,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Machine Learning (practical) - F007 - CL1</t>
+          <t>Cloud Computing (theory) - F008 - AUD2</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Cloud Computing (practical) - F008 - CL1</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD3</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3048,29 +2632,25 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R202</t>
+          <t>Major Project (practical) - F009 - R201</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MDM - Seminar (theory) - F012 - AUD1</t>
+          <t>Major Project (practical) - F009 - R201 (cont.)</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Big Data Analytics (theory) - F022 - R102</t>
         </is>
       </c>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3080,44 +2660,40 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD2</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
+          <t>Artificial Intelligence (theory) - F021 - AUD3</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Lunch Break</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
           <t>Major Project (practical) - F009 - R201</t>
         </is>
       </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>Lunch Break</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - R201 (cont.)</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Big Data Analytics (theory) - F022 - AUD1</t>
         </is>
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3127,12 +2703,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - CL1</t>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD2</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3142,29 +2718,25 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD3</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Big Data Analytics (theory) - F022 - R301</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Artificial Intelligence (practical) - F021 - CL1</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Artificial Intelligence (practical) - F021 - CL1 (cont.)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3188,42 +2760,42 @@
     <row r="1">
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>10:15-11:15</t>
+          <t>10:15 am-11:15 am</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>11:15-12:15</t>
+          <t>11:15 am-12:15 pm</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>12:15-13:15</t>
+          <t>12:15 pm-1:15 pm</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>13:15-14:15</t>
+          <t>1:15 pm-2:15 pm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>14:15-15:15</t>
+          <t>2:15 pm-3:15 pm</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>15:15-15:30</t>
+          <t>3:15 pm-3:30 pm</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>15:30-16:30</t>
+          <t>3:30 pm-4:30 pm</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>16:30-17:30</t>
+          <t>4:30 pm-5:30 pm</t>
         </is>
       </c>
     </row>
@@ -3233,14 +2805,10 @@
           <t>Mon</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Cloud Computing (practical) - F008 - R201</t>
-        </is>
-      </c>
+      <c r="B2" t="inlineStr"/>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Big Data Analytics (theory) - F022 - AUD4</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3250,29 +2818,17 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R201</t>
+          <t>Machine Learning (practical) - F007 - CL1</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>Machine Learning (theory) - F007 - R102</t>
-        </is>
-      </c>
+          <t>Machine Learning (practical) - F007 - CL1 (cont.)</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr"/>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
@@ -3280,16 +2836,8 @@
           <t>Tue</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Machine Learning (practical) - F007 - R202</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Major Project (practical) - F009 - CL1</t>
-        </is>
-      </c>
+      <c r="B3" t="inlineStr"/>
+      <c r="C3" t="inlineStr"/>
       <c r="D3" t="inlineStr">
         <is>
           <t>Lunch Break</t>
@@ -3297,29 +2845,25 @@
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD1</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>MDM - Seminar (theory) - F012 - AUD1</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD1</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Cloud Computing (practical) - F008 - R201</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I3" t="inlineStr">
-        <is>
-          <t>Cloud Computing (theory) - F008 - R101</t>
-        </is>
-      </c>
+          <t>Cloud Computing (practical) - F008 - R201 (cont.)</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
@@ -3329,12 +2873,12 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD4</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R201</t>
+          <t>Machine Learning (theory) - F007 - R301</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -3344,29 +2888,25 @@
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - CL1</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Major Project (practical) - F009 - CL1 (cont.)</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Big Data Analytics (theory) - F022 - R301</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I4" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - R301</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
@@ -3376,12 +2916,12 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - CL2</t>
+          <t>Artificial Intelligence (theory) - F021 - AUD3</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cloud Computing (theory) - F008 - AUD2</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -3391,29 +2931,21 @@
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Big Data Analytics (theory) - F022 - AUD2</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>MDM - Seminar (theory) - F012 - AUD1</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I5" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
@@ -3423,12 +2955,12 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R201</t>
+          <t>Cyber Security (theory) - F023 - AUD3</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Machine Learning (theory) - F007 - AUD2</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -3438,29 +2970,21 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Artificial Intelligence (practical) - F021 - R202</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Cloud Computing (theory) - F008 - AUD1</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>Tea Break</t>
-        </is>
-      </c>
+          <t>Artificial Intelligence (practical) - F021 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr"/>
       <c r="H6" t="inlineStr">
         <is>
-          <t>Machine Learning (theory) - F007 - R101</t>
-        </is>
-      </c>
-      <c r="I6" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R102</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
@@ -3470,12 +2994,12 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Machine Learning (theory) - F007 - AUD1</t>
+          <t>MDM - Seminar (NEP) (theory) - F012 - R101</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Cloud Computing (theory) - F008 - AUD1</t>
+          <t>Cloud Computing (theory) - F008 - AUD3</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
@@ -3485,29 +3009,25 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Major Project (practical) - F009 - R201</t>
+          <t>Machine Learning (theory) - F007 - AUD2</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
+          <t>Cyber Security (theory) - F023 - AUD2</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>Tea Break</t>
+          <t>Major Project (practical) - F009 - R202</t>
         </is>
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
-      <c r="I7" t="inlineStr">
-        <is>
-          <t>Dummy Subject</t>
-        </is>
-      </c>
+          <t>Major Project (practical) - F009 - R202 (cont.)</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>